<commit_message>
Add columns with count of topics and modules in the course
</commit_message>
<xml_diff>
--- a/courses_data.xlsx
+++ b/courses_data.xlsx
@@ -8,16 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="UI_UX designer" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="QA engineer" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Python developer" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Data analyst" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Digital marketer" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Front-end developer" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Full-stack developer" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="DevOps engineer" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet name="Java developer" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet name="Recruiter" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -453,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +454,8 @@
     <col width="22" customWidth="1" min="1" max="1"/>
     <col width="50" customWidth="1" min="2" max="2"/>
     <col width="50" customWidth="1" min="3" max="3"/>
+    <col width="9" customWidth="1" min="4" max="4"/>
+    <col width="8" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -482,6 +474,16 @@
           <t>Description</t>
         </is>
       </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Modules</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Topics</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -499,6 +501,12 @@
           <t>UI/UX-дизайнери спеціалізуються на інтерфейсах додатків. Вони враховують потреби користувачів, їх взаємодії з продуктом та створюють зручний, естетичний та зрозумілий дизайн, який відповідає цим потребам.</t>
         </is>
       </c>
+      <c r="D2" s="3" t="n">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>90</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -516,6 +524,12 @@
           <t>QA-інженер відповідає за розробку планів тестування додатків та сайтів. Тестувальник виявляє недоліки в роботі продукту, а що найважливіше — допомагає уникнути їх у майбутньому.</t>
         </is>
       </c>
+      <c r="D3" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="n">
+        <v>148</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -533,6 +547,12 @@
           <t>Python-розробники можуть працювати в різних сферах: від машинного навчання до веброзробки. Вони володіють знаннями, необхідними для створення, розширення та підтримки програм, які використовують Python як основну мову програмування.</t>
         </is>
       </c>
+      <c r="D4" s="3" t="n">
+        <v>19</v>
+      </c>
+      <c r="E4" s="3" t="n">
+        <v>185</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -550,6 +570,12 @@
           <t>Він допомагає бізнесу приймати рішення на основі даних. Такий підхід дозволяє компаніям розуміти попит на свої продукти, збільшувати продажі, а також краще задовольняти потреби клієнтів.</t>
         </is>
       </c>
+      <c r="D5" s="3" t="n">
+        <v>12</v>
+      </c>
+      <c r="E5" s="3" t="n">
+        <v>40</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -567,6 +593,12 @@
           <t>Використовуй різноманітні маркетингові стратегії, соціальні мережі, пошуковий маркетинг, контент-маркетинг та інші інструменти, щоб рекламувати бренди та залучати цільову аудиторію.</t>
         </is>
       </c>
+      <c r="D6" s="3" t="n">
+        <v>9</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>64</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -584,6 +616,12 @@
           <t>Frontend-розробник відповідає за створення зручного та естетичного вигляду вебсторінки на різних пристроях, а також реалізує анімації та інші інтерфейсні рішення.</t>
         </is>
       </c>
+      <c r="D7" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" s="3" t="n">
+        <v>138</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -601,6 +639,12 @@
           <t>Fullstack-розробники володіють навичками програмування як фронтенду (клієнтська сторона), так і бекенду (серверна сторона). Вони можуть розробити повноцінний продукт від початку до кінця.</t>
         </is>
       </c>
+      <c r="D8" s="3" t="n">
+        <v>25</v>
+      </c>
+      <c r="E8" s="3" t="n">
+        <v>182</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -618,6 +662,12 @@
           <t>DevOps-інженер відповідає за ефективний процес створення програмного продукту, а також виявляє шляхи автоматизації процесів розробки, забезпечуючи надійне та ефективне постачання продукту до кінцевого користувача.</t>
         </is>
       </c>
+      <c r="D9" s="3" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>192</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -635,6 +685,12 @@
           <t>Java-розробники — це творці потужних та надійних додатків, які застосовуються в різних сферах, від роботи банків до агросектору.</t>
         </is>
       </c>
+      <c r="D10" s="3" t="n">
+        <v>16</v>
+      </c>
+      <c r="E10" s="3" t="n">
+        <v>166</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -651,6 +707,12 @@
         <is>
           <t>IT-рекрутери забезпечують розвиток команд. Це експерти у галузі знаходження та відбору кандидатів для вакансій, пов'язаних із розробкою програмного забезпечення, базами даних та іншими IT-напрямками.</t>
         </is>
+      </c>
+      <c r="D11" s="3" t="n">
+        <v>8</v>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -668,184 +730,4 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Update logs and excel file
</commit_message>
<xml_diff>
--- a/courses_data.xlsx
+++ b/courses_data.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,6 +456,8 @@
     <col width="50" customWidth="1" min="3" max="3"/>
     <col width="9" customWidth="1" min="4" max="4"/>
     <col width="8" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="15" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -484,6 +486,16 @@
           <t>Topics</t>
         </is>
       </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>Full-Time Duration</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>Flex Duration</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="inlineStr">
@@ -507,6 +519,16 @@
       <c r="E2" s="3" t="n">
         <v>90</v>
       </c>
+      <c r="F2" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="G2" s="3" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="3" t="inlineStr">
@@ -530,6 +552,16 @@
       <c r="E3" s="3" t="n">
         <v>148</v>
       </c>
+      <c r="F3" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G3" s="3" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="3" t="inlineStr">
@@ -553,6 +585,16 @@
       <c r="E4" s="3" t="n">
         <v>185</v>
       </c>
+      <c r="F4" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
+      <c r="G4" s="3" t="inlineStr">
+        <is>
+          <t>7 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="3" t="inlineStr">
@@ -576,6 +618,16 @@
       <c r="E5" s="3" t="n">
         <v>40</v>
       </c>
+      <c r="F5" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G5" s="3" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="3" t="inlineStr">
@@ -599,6 +651,16 @@
       <c r="E6" s="3" t="n">
         <v>64</v>
       </c>
+      <c r="F6" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G6" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="3" t="inlineStr">
@@ -622,6 +684,16 @@
       <c r="E7" s="3" t="n">
         <v>138</v>
       </c>
+      <c r="F7" s="3" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
+      <c r="G7" s="3" t="inlineStr">
+        <is>
+          <t>7 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="3" t="inlineStr">
@@ -645,6 +717,16 @@
       <c r="E8" s="3" t="n">
         <v>182</v>
       </c>
+      <c r="F8" s="3" t="inlineStr">
+        <is>
+          <t>5 місяців</t>
+        </is>
+      </c>
+      <c r="G8" s="3" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="3" t="inlineStr">
@@ -668,6 +750,16 @@
       <c r="E9" s="3" t="n">
         <v>192</v>
       </c>
+      <c r="F9" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G9" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="3" t="inlineStr">
@@ -691,6 +783,16 @@
       <c r="E10" s="3" t="n">
         <v>166</v>
       </c>
+      <c r="F10" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G10" s="3" t="inlineStr">
+        <is>
+          <t>8 місяців</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="3" t="inlineStr">
@@ -713,6 +815,16 @@
       </c>
       <c r="E11" s="3" t="n">
         <v>45</v>
+      </c>
+      <c r="F11" s="3" t="inlineStr">
+        <is>
+          <t>3 місяці</t>
+        </is>
+      </c>
+      <c r="G11" s="3" t="inlineStr">
+        <is>
+          <t>4 місяці</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>